<commit_message>
Added relay, router, and power supplies to robot model. Made a spreadsheet with the DIN rail layout.
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="19440" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
@@ -136,13 +136,16 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>13.8 v supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,7 +266,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -298,7 +300,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,20 +475,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +502,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -516,7 +517,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -530,7 +531,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -545,7 +546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -559,7 +560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -574,7 +575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -589,7 +590,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -604,7 +605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -619,7 +620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -628,7 +629,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -643,7 +644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -658,7 +659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -673,7 +674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -681,8 +682,14 @@
         <f>13.2/16</f>
         <v>0.82499999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -690,11 +697,14 @@
         <f>7.8/16</f>
         <v>0.48749999999999999</v>
       </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
       <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -703,7 +713,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -711,11 +721,14 @@
         <f>3.2/16</f>
         <v>0.2</v>
       </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
       <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -730,7 +743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -741,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -749,8 +762,14 @@
         <f>10/16</f>
         <v>0.625</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -758,8 +777,14 @@
         <f>1+10.6/16</f>
         <v>1.6625000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -774,7 +799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -789,7 +814,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -804,7 +829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -818,7 +843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -830,12 +855,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -846,7 +871,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -860,7 +885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -868,7 +893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -879,6 +904,17 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
         <v>31</v>
       </c>
     </row>
@@ -888,24 +924,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>